<commit_message>
new format for excel
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Buff.xlsx
+++ b/_Out/NFDataCfg/Excel/Buff.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\NoahGameFrame\_Out\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\NoahGameFrame\_Out\NFDataCfg\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -700,7 +700,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -785,31 +785,31 @@
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="b">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -817,31 +817,31 @@
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2" t="b">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
         <v>0</v>
       </c>
     </row>
@@ -849,31 +849,31 @@
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="b">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -881,31 +881,31 @@
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="b">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
         <v>0</v>
       </c>
     </row>
@@ -913,31 +913,31 @@
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3" t="b">
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -945,31 +945,31 @@
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3" t="b">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
         <v>0</v>
       </c>
     </row>
@@ -977,31 +977,31 @@
       <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3" t="b">
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>